<commit_message>
New software version + new data
</commit_message>
<xml_diff>
--- a/01 - Simulations/Archive - from Senior Project/2nd order active LPF/Wind vane Vout handler.xlsx
+++ b/01 - Simulations/Archive - from Senior Project/2nd order active LPF/Wind vane Vout handler.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Personal Work\Designs\Simulations\2nd order active LPF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5f1ecc3610ff35ee/Senior Project ^0 Bachelor Thesis/Personal works/VGU-WirelessMeteorologyStation/01 - Simulations/Archive - from Senior Project/2nd order active LPF/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7259A55F-0B0F-492B-8C68-84EEFDD34A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{7259A55F-0B0F-492B-8C68-84EEFDD34A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90D0E3FF-EAE3-4E4F-99B9-55FE88A5319B}"/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="1740" windowWidth="21600" windowHeight="11385" xr2:uid="{D87FE679-0198-4AF5-98CF-D95002D7886D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D87FE679-0198-4AF5-98CF-D95002D7886D}"/>
   </bookViews>
   <sheets>
     <sheet name="Wind vane" sheetId="1" r:id="rId1"/>
@@ -23,14 +23,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -404,7 +396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -442,13 +434,10 @@
     <xf numFmtId="168" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="168" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="168" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -494,9 +483,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="168" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -570,7 +556,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -948,7 +934,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1086,52 +1072,52 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>3.0140577716643739</c:v>
+                  <c:v>3.0099175824175823</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2140280027585768</c:v>
+                  <c:v>2.2028069258075447</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.3696590909090909</c:v>
+                  <c:v>2.3593472584856396</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.71331005100264233</c:v>
+                  <c:v>0.70480362989290601</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.78001411100658513</c:v>
+                  <c:v>0.77094839609483956</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.57791042282298921</c:v>
+                  <c:v>0.57066382882436972</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3325183823529412</c:v>
+                  <c:v>1.3203825136612022</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.99649356769071085</c:v>
+                  <c:v>0.98589227501209342</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.8012342215988781</c:v>
+                  <c:v>1.788690807799443</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.6217476139375444</c:v>
+                  <c:v>1.6091210628161745</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.7505876235049405</c:v>
+                  <c:v>2.7434543568464731</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.6898472729684757</c:v>
+                  <c:v>2.6821162865435833</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.2224338624338627</c:v>
+                  <c:v>3.2211228641171683</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.0726359403300658</c:v>
+                  <c:v>3.06924979303276</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.1521496698459281</c:v>
+                  <c:v>3.1498387096774194</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.8826114752968555</c:v>
+                  <c:v>2.876896613111398</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2809,7 +2795,7 @@
   <dimension ref="A1:AC49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+      <selection activeCell="U12" sqref="U12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2825,7 +2811,7 @@
     <col min="12" max="12" width="12.5703125" style="1" customWidth="1"/>
     <col min="13" max="13" width="13.5703125" style="1" customWidth="1"/>
     <col min="14" max="14" width="9.140625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" style="26"/>
+    <col min="15" max="15" width="9.140625" style="25"/>
     <col min="16" max="16" width="3.7109375" style="1" customWidth="1"/>
     <col min="17" max="17" width="16.7109375" style="1" customWidth="1"/>
     <col min="18" max="19" width="12.7109375" style="1" customWidth="1"/>
@@ -2839,17 +2825,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D1" s="22">
+      <c r="D1" s="21">
         <v>5.5</v>
       </c>
-      <c r="E1" s="23">
+      <c r="E1" s="22">
         <v>3300</v>
       </c>
-      <c r="S1" s="22">
+      <c r="S1" s="21">
         <v>3.31</v>
       </c>
-      <c r="T1" s="23">
-        <v>3250</v>
+      <c r="T1" s="22">
+        <v>3300</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
@@ -2859,10 +2845,10 @@
       <c r="J2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="49" t="s">
+      <c r="L2" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="49"/>
+      <c r="M2" s="47"/>
       <c r="X2" s="2" t="s">
         <v>12</v>
       </c>
@@ -2871,7 +2857,7 @@
       </c>
     </row>
     <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="48" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -2898,15 +2884,15 @@
       <c r="J3" s="1">
         <v>0.01</v>
       </c>
-      <c r="L3" s="17">
+      <c r="L3" s="16">
         <v>10</v>
       </c>
-      <c r="M3" s="18">
+      <c r="M3" s="17">
         <f>1000*$D$1/(POWER(2,L3)-1)</f>
         <v>5.376344086021505</v>
       </c>
       <c r="N3" s="6"/>
-      <c r="P3" s="50" t="s">
+      <c r="P3" s="48" t="s">
         <v>15</v>
       </c>
       <c r="Q3" s="4" t="s">
@@ -2933,19 +2919,19 @@
       <c r="Y3" s="1">
         <v>0.01</v>
       </c>
-      <c r="AA3" s="31">
+      <c r="AA3" s="4">
         <v>0</v>
       </c>
-      <c r="AB3" s="31">
+      <c r="AB3" s="4">
         <v>33100</v>
       </c>
       <c r="AC3" s="7">
         <f>S4</f>
-        <v>3.0140577716643739</v>
+        <v>3.0099175824175823</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A4" s="50"/>
+      <c r="A4" s="48"/>
       <c r="B4" s="4">
         <v>0</v>
       </c>
@@ -2974,24 +2960,24 @@
       <c r="J4" s="1">
         <v>0.01</v>
       </c>
-      <c r="L4" s="17">
+      <c r="L4" s="16">
         <v>12</v>
       </c>
-      <c r="M4" s="18">
+      <c r="M4" s="17">
         <f>1000*$D$1/(POWER(2,L4)-1)</f>
         <v>1.343101343101343</v>
       </c>
       <c r="N4" s="6"/>
-      <c r="P4" s="50"/>
-      <c r="Q4" s="19">
+      <c r="P4" s="48"/>
+      <c r="Q4" s="18">
         <v>0</v>
       </c>
-      <c r="R4" s="20">
+      <c r="R4" s="19">
         <v>33100</v>
       </c>
       <c r="S4" s="7">
         <f>$S$1*R4/(R4+$T$1)</f>
-        <v>3.0140577716643739</v>
+        <v>3.0099175824175823</v>
       </c>
       <c r="T4" s="4">
         <f t="shared" ref="T4:T11" si="4">Q4+22.5</f>
@@ -3003,7 +2989,7 @@
       </c>
       <c r="V4" s="7">
         <f>$S$1*U4/(U4+$T$1)</f>
-        <v>2.2140280027585768</v>
+        <v>2.2028069258075447</v>
       </c>
       <c r="X4" s="5">
         <v>560</v>
@@ -3011,7 +2997,7 @@
       <c r="Y4" s="1">
         <v>0.01</v>
       </c>
-      <c r="AA4" s="31">
+      <c r="AA4" s="4">
         <v>22.5</v>
       </c>
       <c r="AB4" s="8">
@@ -3019,11 +3005,11 @@
       </c>
       <c r="AC4" s="7">
         <f>V4</f>
-        <v>2.2140280027585768</v>
+        <v>2.2028069258075447</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A5" s="50"/>
+      <c r="A5" s="48"/>
       <c r="B5" s="4">
         <v>45</v>
       </c>
@@ -3052,23 +3038,23 @@
       <c r="J5" s="1">
         <v>0.01</v>
       </c>
-      <c r="L5" s="17">
+      <c r="L5" s="16">
         <v>16</v>
       </c>
-      <c r="M5" s="18">
+      <c r="M5" s="17">
         <f>1000*$D$1/(POWER(2,L5)-1)</f>
         <v>8.3924620431830313E-2</v>
       </c>
-      <c r="P5" s="50"/>
-      <c r="Q5" s="19">
+      <c r="P5" s="48"/>
+      <c r="Q5" s="18">
         <v>45</v>
       </c>
-      <c r="R5" s="20">
+      <c r="R5" s="19">
         <v>8190</v>
       </c>
       <c r="S5" s="7">
         <f t="shared" ref="S5:S11" si="6">$S$1*R5/(R5+$T$1)</f>
-        <v>2.3696590909090909</v>
+        <v>2.3593472584856396</v>
       </c>
       <c r="T5" s="4">
         <f t="shared" si="4"/>
@@ -3080,7 +3066,7 @@
       </c>
       <c r="V5" s="7">
         <f t="shared" ref="V5:V11" si="7">$S$1*U5/(U5+$T$1)</f>
-        <v>0.71331005100264233</v>
+        <v>0.70480362989290601</v>
       </c>
       <c r="X5" s="5">
         <v>680</v>
@@ -3088,19 +3074,19 @@
       <c r="Y5" s="1">
         <v>0.01</v>
       </c>
-      <c r="AA5" s="31">
+      <c r="AA5" s="4">
         <v>45</v>
       </c>
-      <c r="AB5" s="31">
+      <c r="AB5" s="4">
         <v>8190</v>
       </c>
       <c r="AC5" s="7">
         <f>S5</f>
-        <v>2.3696590909090909</v>
+        <v>2.3593472584856396</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A6" s="50"/>
+      <c r="A6" s="48"/>
       <c r="B6" s="4">
         <v>90</v>
       </c>
@@ -3129,16 +3115,16 @@
       <c r="J6" s="1">
         <v>0.02</v>
       </c>
-      <c r="P6" s="50"/>
-      <c r="Q6" s="19">
+      <c r="P6" s="48"/>
+      <c r="Q6" s="18">
         <v>90</v>
       </c>
-      <c r="R6" s="21">
+      <c r="R6" s="20">
         <v>1002</v>
       </c>
       <c r="S6" s="7">
         <f t="shared" si="6"/>
-        <v>0.78001411100658513</v>
+        <v>0.77094839609483956</v>
       </c>
       <c r="T6" s="4">
         <f t="shared" si="4"/>
@@ -3150,7 +3136,7 @@
       </c>
       <c r="V6" s="7">
         <f t="shared" si="7"/>
-        <v>0.57791042282298921</v>
+        <v>0.57066382882436972</v>
       </c>
       <c r="X6" s="5">
         <v>820</v>
@@ -3158,7 +3144,7 @@
       <c r="Y6" s="1">
         <v>0.02</v>
       </c>
-      <c r="AA6" s="31">
+      <c r="AA6" s="4">
         <v>67.5</v>
       </c>
       <c r="AB6" s="8">
@@ -3166,11 +3152,11 @@
       </c>
       <c r="AC6" s="7">
         <f>V5</f>
-        <v>0.71331005100264233</v>
+        <v>0.70480362989290601</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A7" s="50"/>
+      <c r="A7" s="48"/>
       <c r="B7" s="4">
         <v>135</v>
       </c>
@@ -3199,18 +3185,18 @@
       <c r="J7" s="1">
         <v>0.02</v>
       </c>
-      <c r="P7" s="50"/>
-      <c r="Q7" s="19">
+      <c r="P7" s="48"/>
+      <c r="Q7" s="18">
         <v>135</v>
       </c>
-      <c r="R7" s="20">
+      <c r="R7" s="19">
         <v>2190</v>
       </c>
       <c r="S7" s="7">
         <f t="shared" si="6"/>
-        <v>1.3325183823529412</v>
-      </c>
-      <c r="T7" s="19">
+        <v>1.3203825136612022</v>
+      </c>
+      <c r="T7" s="18">
         <f t="shared" si="4"/>
         <v>157.5</v>
       </c>
@@ -3220,7 +3206,7 @@
       </c>
       <c r="V7" s="7">
         <f t="shared" si="7"/>
-        <v>0.99649356769071085</v>
+        <v>0.98589227501209342</v>
       </c>
       <c r="X7" s="5">
         <v>910</v>
@@ -3228,19 +3214,19 @@
       <c r="Y7" s="1">
         <v>0.02</v>
       </c>
-      <c r="AA7" s="31">
+      <c r="AA7" s="4">
         <v>90</v>
       </c>
-      <c r="AB7" s="31">
+      <c r="AB7" s="4">
         <v>1002</v>
       </c>
       <c r="AC7" s="7">
         <f>S6</f>
-        <v>0.78001411100658513</v>
+        <v>0.77094839609483956</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A8" s="50"/>
+      <c r="A8" s="48"/>
       <c r="B8" s="4">
         <v>180</v>
       </c>
@@ -3269,18 +3255,18 @@
       <c r="J8" s="10">
         <v>0.02</v>
       </c>
-      <c r="P8" s="50"/>
-      <c r="Q8" s="19">
+      <c r="P8" s="48"/>
+      <c r="Q8" s="18">
         <v>180</v>
       </c>
-      <c r="R8" s="20">
+      <c r="R8" s="19">
         <v>3880</v>
       </c>
       <c r="S8" s="7">
         <f t="shared" si="6"/>
-        <v>1.8012342215988781</v>
-      </c>
-      <c r="T8" s="19">
+        <v>1.788690807799443</v>
+      </c>
+      <c r="T8" s="18">
         <f t="shared" si="4"/>
         <v>202.5</v>
       </c>
@@ -3290,7 +3276,7 @@
       </c>
       <c r="V8" s="7">
         <f t="shared" si="7"/>
-        <v>1.6217476139375444</v>
+        <v>1.6091210628161745</v>
       </c>
       <c r="X8" s="9">
         <v>1000</v>
@@ -3298,7 +3284,7 @@
       <c r="Y8" s="10">
         <v>0.02</v>
       </c>
-      <c r="AA8" s="31">
+      <c r="AA8" s="4">
         <v>112.5</v>
       </c>
       <c r="AB8" s="8">
@@ -3306,11 +3292,11 @@
       </c>
       <c r="AC8" s="7">
         <f>V6</f>
-        <v>0.57791042282298921</v>
+        <v>0.57066382882436972</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A9" s="50"/>
+      <c r="A9" s="48"/>
       <c r="B9" s="4">
         <v>225</v>
       </c>
@@ -3339,16 +3325,16 @@
       <c r="J9" s="10">
         <v>0.02</v>
       </c>
-      <c r="P9" s="50"/>
-      <c r="Q9" s="19">
+      <c r="P9" s="48"/>
+      <c r="Q9" s="18">
         <v>225</v>
       </c>
-      <c r="R9" s="20">
+      <c r="R9" s="19">
         <v>15980</v>
       </c>
       <c r="S9" s="7">
         <f t="shared" si="6"/>
-        <v>2.7505876235049405</v>
+        <v>2.7434543568464731</v>
       </c>
       <c r="T9" s="4">
         <f t="shared" si="4"/>
@@ -3360,7 +3346,7 @@
       </c>
       <c r="V9" s="7">
         <f t="shared" si="7"/>
-        <v>2.6898472729684757</v>
+        <v>2.6821162865435833</v>
       </c>
       <c r="X9" s="9">
         <v>1200</v>
@@ -3368,19 +3354,19 @@
       <c r="Y9" s="10">
         <v>0.02</v>
       </c>
-      <c r="AA9" s="31">
+      <c r="AA9" s="4">
         <v>135</v>
       </c>
-      <c r="AB9" s="31">
+      <c r="AB9" s="4">
         <v>2190</v>
       </c>
       <c r="AC9" s="7">
         <f>S7</f>
-        <v>1.3325183823529412</v>
+        <v>1.3203825136612022</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A10" s="50"/>
+      <c r="A10" s="48"/>
       <c r="B10" s="4">
         <v>270</v>
       </c>
@@ -3409,16 +3395,16 @@
       <c r="J10" s="1">
         <v>0.03</v>
       </c>
-      <c r="P10" s="50"/>
-      <c r="Q10" s="19">
+      <c r="P10" s="48"/>
+      <c r="Q10" s="18">
         <v>270</v>
       </c>
-      <c r="R10" s="20">
+      <c r="R10" s="19">
         <v>119600</v>
       </c>
       <c r="S10" s="7">
         <f t="shared" si="6"/>
-        <v>3.2224338624338627</v>
+        <v>3.2211228641171683</v>
       </c>
       <c r="T10" s="4">
         <f t="shared" si="4"/>
@@ -3430,7 +3416,7 @@
       </c>
       <c r="V10" s="7">
         <f t="shared" si="7"/>
-        <v>3.0726359403300658</v>
+        <v>3.06924979303276</v>
       </c>
       <c r="X10" s="9">
         <v>1500</v>
@@ -3438,7 +3424,7 @@
       <c r="Y10" s="1">
         <v>0.03</v>
       </c>
-      <c r="AA10" s="19">
+      <c r="AA10" s="18">
         <v>157.5</v>
       </c>
       <c r="AB10" s="8">
@@ -3446,11 +3432,11 @@
       </c>
       <c r="AC10" s="7">
         <f>V7</f>
-        <v>0.99649356769071085</v>
+        <v>0.98589227501209342</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A11" s="50"/>
+      <c r="A11" s="48"/>
       <c r="B11" s="4">
         <v>315</v>
       </c>
@@ -3479,16 +3465,16 @@
       <c r="J11" s="1">
         <v>0.04</v>
       </c>
-      <c r="P11" s="50"/>
-      <c r="Q11" s="19">
+      <c r="P11" s="48"/>
+      <c r="Q11" s="18">
         <v>315</v>
       </c>
-      <c r="R11" s="20">
+      <c r="R11" s="19">
         <v>64900</v>
       </c>
       <c r="S11" s="7">
-        <f t="shared" si="6"/>
-        <v>3.1521496698459281</v>
+        <f>$S$1*R11/(R11+$T$1)</f>
+        <v>3.1498387096774194</v>
       </c>
       <c r="T11" s="4">
         <f t="shared" si="4"/>
@@ -3500,7 +3486,7 @@
       </c>
       <c r="V11" s="7">
         <f t="shared" si="7"/>
-        <v>2.8826114752968555</v>
+        <v>2.876896613111398</v>
       </c>
       <c r="X11" s="9">
         <v>1800</v>
@@ -3508,15 +3494,15 @@
       <c r="Y11" s="1">
         <v>0.03</v>
       </c>
-      <c r="AA11" s="31">
+      <c r="AA11" s="4">
         <v>180</v>
       </c>
-      <c r="AB11" s="31">
+      <c r="AB11" s="4">
         <v>3880</v>
       </c>
       <c r="AC11" s="7">
         <f>S8</f>
-        <v>1.8012342215988781</v>
+        <v>1.788690807799443</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
@@ -3532,7 +3518,7 @@
       <c r="Y12" s="1">
         <v>0.04</v>
       </c>
-      <c r="AA12" s="19">
+      <c r="AA12" s="18">
         <v>202.5</v>
       </c>
       <c r="AB12" s="8">
@@ -3540,45 +3526,43 @@
       </c>
       <c r="AC12" s="7">
         <f>V8</f>
-        <v>1.6217476139375444</v>
+        <v>1.6091210628161745</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B13" s="49" t="s">
+      <c r="B13" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="13"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="14"/>
       <c r="I13" s="9">
         <v>2200</v>
       </c>
       <c r="J13" s="1">
         <v>0.04</v>
       </c>
-      <c r="Q13" s="49" t="s">
+      <c r="Q13" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="R13" s="49"/>
-      <c r="S13" s="15" t="s">
+      <c r="R13" s="47"/>
+      <c r="S13" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="T13" s="13"/>
       <c r="X13" s="9">
         <v>2200</v>
       </c>
       <c r="Y13" s="1">
         <v>0.04</v>
       </c>
-      <c r="AA13" s="31">
+      <c r="AA13" s="4">
         <v>225</v>
       </c>
-      <c r="AB13" s="31">
+      <c r="AB13" s="4">
         <v>15980</v>
       </c>
       <c r="AC13" s="7">
         <f>S9</f>
-        <v>2.7505876235049405</v>
+        <v>2.7434543568464731</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
@@ -3588,8 +3572,6 @@
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
       <c r="I14" s="9">
         <v>2400</v>
       </c>
@@ -3602,9 +3584,7 @@
       <c r="R14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="S14" s="13"/>
-      <c r="T14" s="13"/>
-      <c r="U14" s="48">
+      <c r="U14" s="46">
         <v>1.5858000000000001</v>
       </c>
       <c r="X14" s="9">
@@ -3613,7 +3593,7 @@
       <c r="Y14" s="1">
         <v>0.05</v>
       </c>
-      <c r="AA14" s="31">
+      <c r="AA14" s="4">
         <v>247.5</v>
       </c>
       <c r="AB14" s="8">
@@ -3621,7 +3601,7 @@
       </c>
       <c r="AC14" s="7">
         <f>V9</f>
-        <v>2.6898472729684757</v>
+        <v>2.6821162865435833</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
@@ -3633,7 +3613,7 @@
       <c r="D15" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="16">
+      <c r="E15" s="15">
         <f>MAX(B15:B30)</f>
         <v>5.3527980535279802</v>
       </c>
@@ -3645,19 +3625,19 @@
       </c>
       <c r="Q15" s="7">
         <f>MAX(S4:S11,V4:V11)</f>
-        <v>3.2224338624338627</v>
+        <v>3.2211228641171683</v>
       </c>
       <c r="R15" s="4"/>
       <c r="S15" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="T15" s="16">
+      <c r="T15" s="15">
         <f>MAX(Q15:Q30)</f>
-        <v>3.2224338624338627</v>
+        <v>3.2211228641171683</v>
       </c>
       <c r="U15" s="1">
         <f>T15*$U$14</f>
-        <v>5.1101356190476199</v>
+        <v>5.1080566379170058</v>
       </c>
       <c r="X15" s="9">
         <v>2700</v>
@@ -3665,15 +3645,15 @@
       <c r="Y15" s="1">
         <v>0.05</v>
       </c>
-      <c r="AA15" s="31">
+      <c r="AA15" s="4">
         <v>270</v>
       </c>
-      <c r="AB15" s="31">
+      <c r="AB15" s="4">
         <v>119600</v>
       </c>
       <c r="AC15" s="7">
         <f>S10</f>
-        <v>3.2224338624338627</v>
+        <v>3.2211228641171683</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
@@ -3692,38 +3672,38 @@
         <f>MIN(B15:B30)</f>
         <v>0.94827586206896552</v>
       </c>
-      <c r="I16" s="27">
+      <c r="I16" s="26">
         <v>3000</v>
       </c>
-      <c r="J16" s="28">
+      <c r="J16" s="27">
         <v>5.5585421985688388E-2</v>
       </c>
       <c r="Q16" s="7">
         <f>MAX(_xlfn.MAXIFS($S$4:$S$11,$S$4:$S$11,"&lt;"&amp;Q15),_xlfn.MAXIFS($V$4:$V$11,$V$4:$V$11,"&lt;"&amp;Q15))</f>
-        <v>3.1521496698459281</v>
+        <v>3.1498387096774194</v>
       </c>
       <c r="R16" s="7">
         <f>Q15-Q16</f>
-        <v>7.0284192587934502E-2</v>
+        <v>7.1284154439748892E-2</v>
       </c>
       <c r="S16" s="4" t="s">
         <v>5</v>
       </c>
       <c r="T16" s="7">
         <f>MIN(Q15:Q30)</f>
-        <v>0.57791042282298921</v>
+        <v>0.57066382882436972</v>
       </c>
       <c r="U16" s="1">
         <f>T16*$U$14</f>
-        <v>0.91645034851269636</v>
-      </c>
-      <c r="X16" s="27">
+        <v>0.90495869974968557</v>
+      </c>
+      <c r="X16" s="26">
         <v>3000</v>
       </c>
-      <c r="Y16" s="29">
+      <c r="Y16" s="28">
         <v>5.4583219775074188E-2</v>
       </c>
-      <c r="AA16" s="31">
+      <c r="AA16" s="4">
         <v>292.5</v>
       </c>
       <c r="AB16" s="8">
@@ -3731,11 +3711,11 @@
       </c>
       <c r="AC16" s="7">
         <f>V10</f>
-        <v>3.0726359403300658</v>
+        <v>3.06924979303276</v>
       </c>
     </row>
     <row r="17" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B17" s="14">
+      <c r="B17" s="13">
         <f t="shared" ref="B17:B30" si="8">MAX(_xlfn.MAXIFS($D$4:$D$11,$D$4:$D$11,"&lt;"&amp;B16),_xlfn.MAXIFS($G$4:$G$11,$G$4:$G$11,"&lt;"&amp;B16))</f>
         <v>5.1003968721757245</v>
       </c>
@@ -3743,39 +3723,35 @@
         <f t="shared" ref="C17:C30" si="9">B16-B17</f>
         <v>0.13347409556621059</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="I17" s="24">
+      <c r="I17" s="23">
         <v>3300</v>
       </c>
-      <c r="J17" s="25">
+      <c r="J17" s="24">
         <v>6.0238123305434321E-2</v>
       </c>
       <c r="Q17" s="7">
         <f t="shared" ref="Q17:Q30" si="10">MAX(_xlfn.MAXIFS($S$4:$S$11,$S$4:$S$11,"&lt;"&amp;Q16),_xlfn.MAXIFS($V$4:$V$11,$V$4:$V$11,"&lt;"&amp;Q16))</f>
-        <v>3.0726359403300658</v>
+        <v>3.06924979303276</v>
       </c>
       <c r="R17" s="7">
         <f t="shared" ref="R17:R30" si="11">Q16-Q17</f>
-        <v>7.951372951586233E-2</v>
-      </c>
-      <c r="S17" s="13"/>
-      <c r="T17" s="13"/>
-      <c r="X17" s="27">
+        <v>8.0588916644659392E-2</v>
+      </c>
+      <c r="X17" s="26">
         <v>3300</v>
       </c>
-      <c r="Y17" s="28">
+      <c r="Y17" s="27">
         <v>5.9152959223590873E-2</v>
       </c>
-      <c r="AA17" s="31">
+      <c r="AA17" s="4">
         <v>315</v>
       </c>
-      <c r="AB17" s="31">
+      <c r="AB17" s="4">
         <v>64900</v>
       </c>
       <c r="AC17" s="7">
         <f>S11</f>
-        <v>3.1521496698459281</v>
+        <v>3.1498387096774194</v>
       </c>
     </row>
     <row r="18" spans="2:29" x14ac:dyDescent="0.25">
@@ -3794,38 +3770,38 @@
         <f>AVERAGE(C16:C30)</f>
         <v>0.29363481276393427</v>
       </c>
-      <c r="I18" s="27">
+      <c r="I18" s="26">
         <v>3900</v>
       </c>
-      <c r="J18" s="28">
+      <c r="J18" s="27">
         <v>5.95855402051928E-2</v>
       </c>
       <c r="Q18" s="7">
         <f t="shared" si="10"/>
-        <v>3.0140577716643739</v>
+        <v>3.0099175824175823</v>
       </c>
       <c r="R18" s="7">
         <f t="shared" si="11"/>
-        <v>5.8578168665691877E-2</v>
+        <v>5.9332210615177683E-2</v>
       </c>
       <c r="S18" s="4" t="s">
         <v>8</v>
       </c>
       <c r="T18" s="7">
         <f>AVERAGE(R16:R30)</f>
-        <v>0.17630156264072488</v>
+        <v>0.1766972690195199</v>
       </c>
       <c r="U18" s="1">
         <f>T18*$U$14</f>
-        <v>0.27957901803566154</v>
-      </c>
-      <c r="X18" s="24">
+        <v>0.28020652921115469</v>
+      </c>
+      <c r="X18" s="23">
         <v>3900</v>
       </c>
-      <c r="Y18" s="30">
+      <c r="Y18" s="29">
         <v>5.9833402885865583E-2</v>
       </c>
-      <c r="AA18" s="31">
+      <c r="AA18" s="4">
         <v>337.5</v>
       </c>
       <c r="AB18" s="8">
@@ -3833,7 +3809,7 @@
       </c>
       <c r="AC18" s="7">
         <f>V11</f>
-        <v>2.8826114752968555</v>
+        <v>2.876896613111398</v>
       </c>
     </row>
     <row r="19" spans="2:29" x14ac:dyDescent="0.25">
@@ -3860,22 +3836,22 @@
       </c>
       <c r="Q19" s="7">
         <f t="shared" si="10"/>
-        <v>2.8826114752968555</v>
+        <v>2.876896613111398</v>
       </c>
       <c r="R19" s="7">
         <f t="shared" si="11"/>
-        <v>0.13144629636751848</v>
+        <v>0.13302096930618434</v>
       </c>
       <c r="S19" s="4" t="s">
         <v>10</v>
       </c>
       <c r="T19" s="7">
         <f>MAX(R16:R30)</f>
-        <v>0.41279378115969867</v>
+        <v>0.41411611800810166</v>
       </c>
       <c r="U19" s="1">
         <f t="shared" ref="U19:U20" si="12">T19*$U$14</f>
-        <v>0.65460837816305018</v>
+        <v>0.65670533993724767</v>
       </c>
       <c r="X19" s="9">
         <v>4700</v>
@@ -3908,22 +3884,22 @@
       </c>
       <c r="Q20" s="7">
         <f t="shared" si="10"/>
-        <v>2.7505876235049405</v>
+        <v>2.7434543568464731</v>
       </c>
       <c r="R20" s="7">
         <f t="shared" si="11"/>
-        <v>0.132023851791915</v>
+        <v>0.1334422562649249</v>
       </c>
       <c r="S20" s="11" t="s">
         <v>11</v>
       </c>
       <c r="T20" s="12">
         <f>MIN(R16:R30)</f>
-        <v>5.8578168665691877E-2</v>
+        <v>5.9332210615177683E-2</v>
       </c>
       <c r="U20" s="1">
         <f t="shared" si="12"/>
-        <v>9.2893259870054187E-2</v>
+        <v>9.4089019593548776E-2</v>
       </c>
       <c r="X20" s="9">
         <v>5100</v>
@@ -3941,8 +3917,6 @@
         <f t="shared" si="9"/>
         <v>0.10163209810437301</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
       <c r="I21" s="9">
         <v>5600</v>
       </c>
@@ -3951,14 +3925,12 @@
       </c>
       <c r="Q21" s="7">
         <f t="shared" si="10"/>
-        <v>2.6898472729684757</v>
+        <v>2.6821162865435833</v>
       </c>
       <c r="R21" s="7">
         <f t="shared" si="11"/>
-        <v>6.074035053646476E-2</v>
-      </c>
-      <c r="S21" s="13"/>
-      <c r="T21" s="13"/>
+        <v>6.1338070302889847E-2</v>
+      </c>
       <c r="X21" s="9">
         <v>5600</v>
       </c>
@@ -3975,8 +3947,6 @@
         <f t="shared" si="9"/>
         <v>0.53621426368882386</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
       <c r="I22" s="9">
         <v>6800</v>
       </c>
@@ -3985,14 +3955,12 @@
       </c>
       <c r="Q22" s="7">
         <f t="shared" si="10"/>
-        <v>2.3696590909090909</v>
+        <v>2.3593472584856396</v>
       </c>
       <c r="R22" s="7">
         <f t="shared" si="11"/>
-        <v>0.32018818205938482</v>
-      </c>
-      <c r="S22" s="13"/>
-      <c r="T22" s="13"/>
+        <v>0.32276902805794361</v>
+      </c>
       <c r="X22" s="9">
         <v>6800</v>
       </c>
@@ -4009,8 +3977,6 @@
         <f t="shared" si="9"/>
         <v>0.26102484472049658</v>
       </c>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
       <c r="I23" s="9">
         <v>7500</v>
       </c>
@@ -4019,14 +3985,12 @@
       </c>
       <c r="Q23" s="7">
         <f t="shared" si="10"/>
-        <v>2.2140280027585768</v>
+        <v>2.2028069258075447</v>
       </c>
       <c r="R23" s="7">
         <f t="shared" si="11"/>
-        <v>0.15563108815051407</v>
-      </c>
-      <c r="S23" s="13"/>
-      <c r="T23" s="13"/>
+        <v>0.15654033267809497</v>
+      </c>
       <c r="X23" s="9">
         <v>7500</v>
       </c>
@@ -4043,8 +4007,6 @@
         <f t="shared" si="9"/>
         <v>0.68154761904761951</v>
       </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
       <c r="I24" s="9">
         <v>8200</v>
       </c>
@@ -4053,14 +4015,12 @@
       </c>
       <c r="Q24" s="7">
         <f t="shared" si="10"/>
-        <v>1.8012342215988781</v>
+        <v>1.788690807799443</v>
       </c>
       <c r="R24" s="7">
         <f t="shared" si="11"/>
-        <v>0.41279378115969867</v>
-      </c>
-      <c r="S24" s="13"/>
-      <c r="T24" s="13"/>
+        <v>0.41411611800810166</v>
+      </c>
       <c r="X24" s="9">
         <v>8200</v>
       </c>
@@ -4077,8 +4037,6 @@
         <f t="shared" si="9"/>
         <v>0.29938217381119703</v>
       </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
       <c r="I25" s="9">
         <v>10000</v>
       </c>
@@ -4087,14 +4045,12 @@
       </c>
       <c r="Q25" s="7">
         <f t="shared" si="10"/>
-        <v>1.6217476139375444</v>
+        <v>1.6091210628161745</v>
       </c>
       <c r="R25" s="7">
         <f t="shared" si="11"/>
-        <v>0.17948660766133373</v>
-      </c>
-      <c r="S25" s="13"/>
-      <c r="T25" s="13"/>
+        <v>0.1795697449832685</v>
+      </c>
       <c r="X25" s="9">
         <v>10000</v>
       </c>
@@ -4111,8 +4067,6 @@
         <f t="shared" si="9"/>
         <v>0.47978449285546931</v>
       </c>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
       <c r="I26" s="9">
         <v>12000</v>
       </c>
@@ -4121,14 +4075,12 @@
       </c>
       <c r="Q26" s="7">
         <f t="shared" si="10"/>
-        <v>1.3325183823529412</v>
+        <v>1.3203825136612022</v>
       </c>
       <c r="R26" s="7">
         <f t="shared" si="11"/>
-        <v>0.28922923158460323</v>
-      </c>
-      <c r="S26" s="13"/>
-      <c r="T26" s="13"/>
+        <v>0.28873854915497232</v>
+      </c>
       <c r="X26" s="9">
         <v>12000</v>
       </c>
@@ -4145,8 +4097,6 @@
         <f t="shared" si="9"/>
         <v>0.55632183908045985</v>
       </c>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
       <c r="I27" s="9">
         <v>13000</v>
       </c>
@@ -4155,14 +4105,12 @@
       </c>
       <c r="Q27" s="7">
         <f t="shared" si="10"/>
-        <v>0.99649356769071085</v>
+        <v>0.98589227501209342</v>
       </c>
       <c r="R27" s="7">
         <f t="shared" si="11"/>
-        <v>0.33602481466223033</v>
-      </c>
-      <c r="S27" s="13"/>
-      <c r="T27" s="13"/>
+        <v>0.33449023864910876</v>
+      </c>
       <c r="X27" s="9">
         <v>13000</v>
       </c>
@@ -4179,8 +4127,6 @@
         <f t="shared" si="9"/>
         <v>0.36460839347767982</v>
       </c>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
       <c r="I28" s="9">
         <v>15000</v>
       </c>
@@ -4189,14 +4135,12 @@
       </c>
       <c r="Q28" s="7">
         <f t="shared" si="10"/>
-        <v>0.78001411100658513</v>
+        <v>0.77094839609483956</v>
       </c>
       <c r="R28" s="7">
         <f t="shared" si="11"/>
-        <v>0.21647945668412572</v>
-      </c>
-      <c r="S28" s="13"/>
-      <c r="T28" s="13"/>
+        <v>0.21494387891725386</v>
+      </c>
       <c r="X28" s="9">
         <v>15000</v>
       </c>
@@ -4213,8 +4157,6 @@
         <f t="shared" si="9"/>
         <v>0.10946395831322997</v>
       </c>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
       <c r="I29" s="9">
         <v>18000</v>
       </c>
@@ -4223,14 +4165,12 @@
       </c>
       <c r="Q29" s="7">
         <f t="shared" si="10"/>
-        <v>0.71331005100264233</v>
+        <v>0.70480362989290601</v>
       </c>
       <c r="R29" s="7">
         <f t="shared" si="11"/>
-        <v>6.67040600039428E-2</v>
-      </c>
-      <c r="S29" s="13"/>
-      <c r="T29" s="13"/>
+        <v>6.6144766201933547E-2</v>
+      </c>
       <c r="X29" s="9">
         <v>18000</v>
       </c>
@@ -4247,8 +4187,6 @@
         <f t="shared" si="9"/>
         <v>0.22132994705966502</v>
       </c>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
       <c r="I30" s="9">
         <v>20000</v>
       </c>
@@ -4257,14 +4195,12 @@
       </c>
       <c r="Q30" s="7">
         <f t="shared" si="10"/>
-        <v>0.57791042282298921</v>
+        <v>0.57066382882436972</v>
       </c>
       <c r="R30" s="7">
         <f t="shared" si="11"/>
-        <v>0.13539962817965312</v>
-      </c>
-      <c r="S30" s="13"/>
-      <c r="T30" s="13"/>
+        <v>0.13413980106853629</v>
+      </c>
       <c r="X30" s="9">
         <v>20000</v>
       </c>
@@ -4293,14 +4229,13 @@
       <c r="J32" s="1">
         <v>0.01</v>
       </c>
-      <c r="Q32" s="49" t="s">
+      <c r="Q32" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="R32" s="49"/>
-      <c r="S32" s="15" t="s">
+      <c r="R32" s="47"/>
+      <c r="S32" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="T32" s="13"/>
       <c r="X32" s="9">
         <v>24000</v>
       </c>
@@ -4315,14 +4250,12 @@
       <c r="J33" s="1">
         <v>0.01</v>
       </c>
-      <c r="Q33" s="31" t="s">
+      <c r="Q33" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="R33" s="31" t="s">
+      <c r="R33" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="S33" s="13"/>
-      <c r="T33" s="13"/>
       <c r="X33" s="9">
         <v>27000</v>
       </c>
@@ -4341,11 +4274,11 @@
         <f>MAX(R4:R11,U4:U11)</f>
         <v>119600</v>
       </c>
-      <c r="R34" s="31"/>
-      <c r="S34" s="31" t="s">
+      <c r="R34" s="4"/>
+      <c r="S34" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="T34" s="46">
+      <c r="T34" s="44">
         <f>MAX(Q34:Q49)</f>
         <v>119600</v>
       </c>
@@ -4367,14 +4300,14 @@
         <f>MAX(_xlfn.MAXIFS($R$4:$R$11,$R$4:$R$11,"&lt;"&amp;Q34),_xlfn.MAXIFS($U$4:$U$11,$U$4:$U$11,"&lt;"&amp;Q34))</f>
         <v>64900</v>
       </c>
-      <c r="R35" s="45">
+      <c r="R35" s="43">
         <f>Q34-Q35</f>
         <v>54700</v>
       </c>
-      <c r="S35" s="31" t="s">
+      <c r="S35" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="T35" s="45">
+      <c r="T35" s="43">
         <f>MIN(Q34:Q49)</f>
         <v>687.46240601503769</v>
       </c>
@@ -4396,12 +4329,10 @@
         <f t="shared" ref="Q36:Q49" si="13">MAX(_xlfn.MAXIFS($R$4:$R$11,$R$4:$R$11,"&lt;"&amp;Q35),_xlfn.MAXIFS($U$4:$U$11,$U$4:$U$11,"&lt;"&amp;Q35))</f>
         <v>42070.677506775071</v>
       </c>
-      <c r="R36" s="45">
+      <c r="R36" s="43">
         <f t="shared" ref="R36:R49" si="14">Q35-Q36</f>
         <v>22829.322493224929</v>
       </c>
-      <c r="S36" s="13"/>
-      <c r="T36" s="13"/>
       <c r="X36" s="9">
         <v>36000</v>
       </c>
@@ -4420,14 +4351,14 @@
         <f t="shared" si="13"/>
         <v>33100</v>
       </c>
-      <c r="R37" s="45">
+      <c r="R37" s="43">
         <f t="shared" si="14"/>
         <v>8970.6775067750714</v>
       </c>
-      <c r="S37" s="31" t="s">
+      <c r="S37" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="T37" s="45">
+      <c r="T37" s="43">
         <f>AVERAGE(R35:R49)</f>
         <v>7927.502506265665</v>
       </c>
@@ -4449,14 +4380,14 @@
         <f t="shared" si="13"/>
         <v>21920.306122448979</v>
       </c>
-      <c r="R38" s="45">
+      <c r="R38" s="43">
         <f t="shared" si="14"/>
         <v>11179.693877551021</v>
       </c>
-      <c r="S38" s="31" t="s">
+      <c r="S38" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="T38" s="45">
+      <c r="T38" s="43">
         <f>MAX(R35:R49)</f>
         <v>54700</v>
       </c>
@@ -4472,14 +4403,14 @@
         <f t="shared" si="13"/>
         <v>15980</v>
       </c>
-      <c r="R39" s="45">
+      <c r="R39" s="43">
         <f t="shared" si="14"/>
         <v>5940.3061224489793</v>
       </c>
       <c r="S39" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="T39" s="47">
+      <c r="T39" s="45">
         <f>MIN(R35:R49)</f>
         <v>109.22584856396861</v>
       </c>
@@ -4489,120 +4420,100 @@
         <f t="shared" si="13"/>
         <v>14096.533412007671</v>
       </c>
-      <c r="R40" s="45">
+      <c r="R40" s="43">
         <f t="shared" si="14"/>
         <v>1883.4665879923286</v>
       </c>
-      <c r="S40" s="13"/>
-      <c r="T40" s="13"/>
     </row>
     <row r="41" spans="9:25" x14ac:dyDescent="0.25">
       <c r="Q41" s="8">
         <f t="shared" si="13"/>
         <v>8190</v>
       </c>
-      <c r="R41" s="45">
+      <c r="R41" s="43">
         <f t="shared" si="14"/>
         <v>5906.5334120076714</v>
       </c>
-      <c r="S41" s="13"/>
-      <c r="T41" s="13"/>
     </row>
     <row r="42" spans="9:25" x14ac:dyDescent="0.25">
       <c r="Q42" s="8">
         <f t="shared" si="13"/>
         <v>6565.4880116250906</v>
       </c>
-      <c r="R42" s="45">
+      <c r="R42" s="43">
         <f t="shared" si="14"/>
         <v>1624.5119883749094</v>
       </c>
-      <c r="S42" s="13"/>
-      <c r="T42" s="13"/>
     </row>
     <row r="43" spans="9:25" x14ac:dyDescent="0.25">
       <c r="Q43" s="8">
         <f t="shared" si="13"/>
         <v>3880</v>
       </c>
-      <c r="R43" s="45">
+      <c r="R43" s="43">
         <f t="shared" si="14"/>
         <v>2685.4880116250906</v>
       </c>
-      <c r="S43" s="13"/>
-      <c r="T43" s="13"/>
     </row>
     <row r="44" spans="9:25" x14ac:dyDescent="0.25">
       <c r="Q44" s="8">
         <f t="shared" si="13"/>
         <v>3121.973816717019</v>
       </c>
-      <c r="R44" s="45">
+      <c r="R44" s="43">
         <f t="shared" si="14"/>
         <v>758.02618328298104</v>
       </c>
-      <c r="S44" s="13"/>
-      <c r="T44" s="13"/>
     </row>
     <row r="45" spans="9:25" x14ac:dyDescent="0.25">
       <c r="Q45" s="8">
         <f t="shared" si="13"/>
         <v>2190</v>
       </c>
-      <c r="R45" s="45">
+      <c r="R45" s="43">
         <f t="shared" si="14"/>
         <v>931.97381671701896</v>
       </c>
-      <c r="S45" s="13"/>
-      <c r="T45" s="13"/>
     </row>
     <row r="46" spans="9:25" x14ac:dyDescent="0.25">
       <c r="Q46" s="8">
         <f t="shared" si="13"/>
         <v>1399.8682042833609</v>
       </c>
-      <c r="R46" s="45">
+      <c r="R46" s="43">
         <f t="shared" si="14"/>
         <v>790.13179571663909</v>
       </c>
-      <c r="S46" s="13"/>
-      <c r="T46" s="13"/>
     </row>
     <row r="47" spans="9:25" x14ac:dyDescent="0.25">
       <c r="Q47" s="8">
         <f t="shared" si="13"/>
         <v>1002</v>
       </c>
-      <c r="R47" s="45">
+      <c r="R47" s="43">
         <f t="shared" si="14"/>
         <v>397.86820428336091</v>
       </c>
-      <c r="S47" s="13"/>
-      <c r="T47" s="13"/>
     </row>
     <row r="48" spans="9:25" x14ac:dyDescent="0.25">
       <c r="Q48" s="8">
         <f t="shared" si="13"/>
         <v>892.77415143603139</v>
       </c>
-      <c r="R48" s="45">
+      <c r="R48" s="43">
         <f t="shared" si="14"/>
         <v>109.22584856396861</v>
       </c>
-      <c r="S48" s="13"/>
-      <c r="T48" s="13"/>
-    </row>
-    <row r="49" spans="17:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="17:18" x14ac:dyDescent="0.25">
       <c r="Q49" s="8">
         <f t="shared" si="13"/>
         <v>687.46240601503769</v>
       </c>
-      <c r="R49" s="45">
+      <c r="R49" s="43">
         <f t="shared" si="14"/>
         <v>205.3117454209937</v>
       </c>
-      <c r="S49" s="13"/>
-      <c r="T49" s="13"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="AA3:AC18">
@@ -4632,298 +4543,298 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="34"/>
-    <col min="2" max="2" width="13.42578125" style="34" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="32"/>
+    <col min="2" max="2" width="13.42578125" style="32" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.85546875" customWidth="1"/>
     <col min="8" max="8" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="33" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="36">
+      <c r="B4" s="34">
         <v>2000</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="33" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A6" s="37" t="s">
+    <row r="6" spans="1:8" s="31" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A6" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="37" t="s">
+      <c r="D6" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="37" t="s">
+      <c r="E6" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="37" t="s">
+      <c r="F6" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="37" t="s">
+      <c r="G6" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="37" t="s">
+      <c r="H6" s="35" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="38">
+      <c r="A7" s="36">
         <v>4.7</v>
       </c>
-      <c r="B7" s="39">
+      <c r="B7" s="37">
         <f>1/(2*PI()*$B$4*A7)</f>
         <v>1.6931376924669717E-5</v>
       </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="38">
+      <c r="A8" s="36">
         <v>68</v>
       </c>
-      <c r="B8" s="39">
+      <c r="B8" s="37">
         <f t="shared" ref="B8:B25" si="0">1/(2*PI()*$B$4*A8)</f>
         <v>1.1702569344992305E-6</v>
       </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="38">
+      <c r="A9" s="36">
         <v>100</v>
       </c>
-      <c r="B9" s="39">
+      <c r="B9" s="37">
         <f t="shared" si="0"/>
         <v>7.9577471545947677E-7</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="38">
+      <c r="A10" s="36">
         <v>150</v>
       </c>
-      <c r="B10" s="39">
+      <c r="B10" s="37">
         <f t="shared" si="0"/>
         <v>5.3051647697298451E-7</v>
       </c>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="38">
+      <c r="A11" s="36">
         <v>180</v>
       </c>
-      <c r="B11" s="39">
+      <c r="B11" s="37">
         <f t="shared" si="0"/>
         <v>4.420970641441538E-7</v>
       </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="38">
+      <c r="A12" s="36">
         <v>330</v>
       </c>
-      <c r="B12" s="39">
+      <c r="B12" s="37">
         <f t="shared" si="0"/>
         <v>2.4114385316953841E-7</v>
       </c>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="38">
+      <c r="A13" s="36">
         <v>350</v>
       </c>
-      <c r="B13" s="39">
+      <c r="B13" s="37">
         <f t="shared" si="0"/>
         <v>2.2736420441699336E-7</v>
       </c>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="38">
+      <c r="A14" s="36">
         <v>390</v>
       </c>
-      <c r="B14" s="39">
+      <c r="B14" s="37">
         <f t="shared" si="0"/>
         <v>2.0404479883576326E-7</v>
       </c>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="38">
+      <c r="A15" s="36">
         <v>470</v>
       </c>
-      <c r="B15" s="39">
+      <c r="B15" s="37">
         <f t="shared" si="0"/>
         <v>1.6931376924669719E-7</v>
       </c>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="41">
+      <c r="A16" s="39">
         <v>560</v>
       </c>
-      <c r="B16" s="42">
+      <c r="B16" s="40">
         <f t="shared" si="0"/>
         <v>1.4210262776062085E-7</v>
       </c>
-      <c r="C16" s="43"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="41">
+      <c r="A17" s="39">
         <v>680</v>
       </c>
-      <c r="B17" s="42">
+      <c r="B17" s="40">
         <f t="shared" si="0"/>
         <v>1.1702569344992305E-7</v>
       </c>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="41">
+      <c r="A18" s="39">
         <v>820</v>
       </c>
-      <c r="B18" s="42">
+      <c r="B18" s="40">
         <f t="shared" si="0"/>
         <v>9.7045697007253269E-8</v>
       </c>
-      <c r="C18" s="43"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="41">
+      <c r="A19" s="39">
         <v>1000</v>
       </c>
-      <c r="B19" s="42">
+      <c r="B19" s="40">
         <f t="shared" si="0"/>
         <v>7.9577471545947674E-8</v>
       </c>
-      <c r="C19" s="43"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="41">
+      <c r="A20" s="39">
         <v>1200</v>
       </c>
-      <c r="B20" s="42">
+      <c r="B20" s="40">
         <f t="shared" si="0"/>
         <v>6.6314559621623064E-8</v>
       </c>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="43"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="41">
+      <c r="A21" s="39">
         <v>2200</v>
       </c>
-      <c r="B21" s="42">
+      <c r="B21" s="40">
         <f t="shared" si="0"/>
         <v>3.6171577975430763E-8</v>
       </c>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="41"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="41">
+      <c r="A22" s="39">
         <v>3300</v>
       </c>
-      <c r="B22" s="42">
+      <c r="B22" s="40">
         <f t="shared" si="0"/>
         <v>2.4114385316953843E-8</v>
       </c>
-      <c r="C22" s="43"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="43"/>
-      <c r="F22" s="43"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="41"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="41">
+      <c r="A23" s="39">
         <v>4700</v>
       </c>
-      <c r="B23" s="42">
+      <c r="B23" s="40">
         <f t="shared" si="0"/>
         <v>1.6931376924669719E-8</v>
       </c>
-      <c r="C23" s="43"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="43"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="41"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="38">
+      <c r="A24" s="36">
         <v>8200</v>
       </c>
-      <c r="B24" s="39">
+      <c r="B24" s="37">
         <f t="shared" si="0"/>
         <v>9.7045697007253266E-9</v>
       </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="38">
+      <c r="A25" s="36">
         <v>10000</v>
       </c>
-      <c r="B25" s="38">
+      <c r="B25" s="36">
         <f t="shared" si="0"/>
         <v>7.9577471545947671E-9</v>
       </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
-      <c r="F25" s="40"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:A24">

</xml_diff>